<commit_message>
dodany atrybut w encji EMPLOYEE i rozpoczęta dokumentacja
</commit_message>
<xml_diff>
--- a/first/TrafficSchool.xlsx
+++ b/first/TrafficSchool.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{63F7DDBC-1CF3-42D9-8187-5E80B4E982FB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4B4FE645-27DC-4BC6-9F32-8C417066DE3D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>PERSON</t>
   </si>
@@ -367,24 +367,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,6 +378,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -682,36 +682,36 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -727,21 +727,22 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -753,26 +754,29 @@
       <c r="E8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -781,7 +785,7 @@
       <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -791,31 +795,31 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -825,21 +829,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -855,19 +859,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="14" t="s">
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -877,31 +881,31 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G31" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="10"/>
-      <c r="J32" s="7" t="s">
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="4"/>
+      <c r="J32" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="K32" s="9"/>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="14" t="s">
+      <c r="K32" s="14"/>
+    </row>
+    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -919,27 +923,27 @@
       <c r="G33" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="J33" s="8" t="s">
         <v>25</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="14" t="s">
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="11"/>
+    </row>
+    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -952,25 +956,25 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="6"/>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="14" t="s">
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="11"/>
+    </row>
+    <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -979,7 +983,7 @@
       <c r="D43" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F43" s="2" t="s">
@@ -1008,8 +1012,8 @@
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="J32:K32"/>
     <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B7:F7"/>
     <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sql tworzacy tabele i zwiazki
</commit_message>
<xml_diff>
--- a/first/TrafficSchool.xlsx
+++ b/first/TrafficSchool.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4B4FE645-27DC-4BC6-9F32-8C417066DE3D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8572F056-A40C-49CE-9947-927475DEC07F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
   <si>
     <t>PERSON</t>
   </si>
@@ -40,36 +40,21 @@
     <t>EMPLOYEE</t>
   </si>
   <si>
-    <t>EmploymentDate</t>
-  </si>
-  <si>
     <t>Salary</t>
   </si>
   <si>
     <t>TRAINEE</t>
   </si>
   <si>
-    <t>StartingDate</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
     <t>Theory</t>
   </si>
   <si>
-    <t>InternalExam</t>
-  </si>
-  <si>
     <t>POSITION</t>
   </si>
   <si>
-    <t>FinishDate</t>
-  </si>
-  <si>
-    <t>BasicSalary</t>
-  </si>
-  <si>
     <t>Overtime</t>
   </si>
   <si>
@@ -82,33 +67,18 @@
     <t>Street</t>
   </si>
   <si>
-    <t>BuildingNumber</t>
-  </si>
-  <si>
-    <t>FlatNumber</t>
-  </si>
-  <si>
     <t>WORD</t>
   </si>
   <si>
     <t>EXAM</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
     <t>VEHICLE</t>
   </si>
   <si>
-    <t>NumberPlate</t>
-  </si>
-  <si>
     <t>Brand</t>
   </si>
   <si>
@@ -118,15 +88,6 @@
     <t>LESSON</t>
   </si>
   <si>
-    <t>FinishTime</t>
-  </si>
-  <si>
-    <t>HowLong</t>
-  </si>
-  <si>
-    <t>Where</t>
-  </si>
-  <si>
     <t>ID_addr</t>
   </si>
   <si>
@@ -139,9 +100,6 @@
     <t>ID_word</t>
   </si>
   <si>
-    <t>Pass/Not</t>
-  </si>
-  <si>
     <t>ID_exam</t>
   </si>
   <si>
@@ -151,22 +109,88 @@
     <t>ID_lesson</t>
   </si>
   <si>
-    <t>NameOfPosition</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
-    <t>ID_pos</t>
-  </si>
-  <si>
     <t>EXAM_TYPE</t>
   </si>
   <si>
-    <t>StartingTime</t>
-  </si>
-  <si>
     <t>trainee will inform school about his exams (pass or not)</t>
+  </si>
+  <si>
+    <t>POSITION_DATA</t>
+  </si>
+  <si>
+    <t>Employment_date</t>
+  </si>
+  <si>
+    <t>Name_of_position</t>
+  </si>
+  <si>
+    <t>Starting_time</t>
+  </si>
+  <si>
+    <t>Starting_date</t>
+  </si>
+  <si>
+    <t>Internal_exam</t>
+  </si>
+  <si>
+    <t>Basic_salary</t>
+  </si>
+  <si>
+    <t>Finish_date</t>
+  </si>
+  <si>
+    <t>Building_number</t>
+  </si>
+  <si>
+    <t>Flat_number</t>
+  </si>
+  <si>
+    <t>Number_plate</t>
+  </si>
+  <si>
+    <t>Finish_time</t>
+  </si>
+  <si>
+    <t>How_long</t>
+  </si>
+  <si>
+    <t>AREA</t>
+  </si>
+  <si>
+    <t>pass/not/(scheduled)</t>
+  </si>
+  <si>
+    <t>(n)</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>E_type</t>
+  </si>
+  <si>
+    <t>E_date</t>
+  </si>
+  <si>
+    <t>L_date</t>
+  </si>
+  <si>
+    <t>Pass_or_not</t>
+  </si>
+  <si>
+    <t>Area_name</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>B-C?</t>
+  </si>
+  <si>
+    <t>czy to jest w P. Boyce'a Codd'a? (ID_emp vs PESEL)</t>
   </si>
 </sst>
 </file>
@@ -191,7 +215,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,24 +230,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -352,11 +382,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,13 +429,37 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -392,10 +474,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -678,342 +760,416 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="8" t="s">
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="F13" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
+        <v>29</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="21"/>
     </row>
     <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>14</v>
+      <c r="B18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>16</v>
+        <v>35</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <f>"(7)"</f>
+        <v>(7)</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="11"/>
+        <v>29</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="19"/>
     </row>
     <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>18</v>
+      <c r="B23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>21</v>
+        <v>36</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="11"/>
+        <v>29</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="19"/>
     </row>
     <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="8" t="s">
-        <v>38</v>
+      <c r="B28" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>35</v>
+      <c r="D28" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G31" s="1" t="s">
-        <v>48</v>
+      <c r="K31" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="21"/>
+      <c r="F32" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="19"/>
+    </row>
+    <row r="33" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K34" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="19"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C39" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="19"/>
+      <c r="F42" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="19"/>
+    </row>
+    <row r="43" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="F43" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J43" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="K43" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="4"/>
-      <c r="J32" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="K32" s="14"/>
-    </row>
-    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="L43" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="9" t="s">
+      <c r="M43" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
-    </row>
-    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="11"/>
-    </row>
-    <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J43" s="3" t="s">
-        <v>41</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="F42:M42"/>
     <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B12:F12"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B22:F22"/>
     <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B32:C32"/>
     <mergeCell ref="B17:G17"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="E7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
obrazki i skrypt kursanta (ale bedzie jeszcze zmieniane)
</commit_message>
<xml_diff>
--- a/first/TrafficSchool.xlsx
+++ b/first/TrafficSchool.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8572F056-A40C-49CE-9947-927475DEC07F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{07188FDE-DDF4-45C7-A62D-F895EAB70FF6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t>PERSON</t>
   </si>
@@ -121,9 +121,6 @@
     <t>POSITION_DATA</t>
   </si>
   <si>
-    <t>Employment_date</t>
-  </si>
-  <si>
     <t>Name_of_position</t>
   </si>
   <si>
@@ -191,18 +188,47 @@
   </si>
   <si>
     <t>czy to jest w P. Boyce'a Codd'a? (ID_emp vs PESEL)</t>
+  </si>
+  <si>
+    <t>Hire_date</t>
+  </si>
+  <si>
+    <t>no dobra, ale jaka to pensja? Miesieczna? Roczna? Przeciez nie ma historii. To będzie jako zapytnie</t>
+  </si>
+  <si>
+    <t>emp Y</t>
+  </si>
+  <si>
+    <t>script N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>scriptTRN N</t>
+  </si>
+  <si>
+    <t>word_emp Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -416,69 +442,71 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -760,416 +788,462 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="7.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="19"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="11" t="s">
+      <c r="G2" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="G3" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="17" t="s">
+      <c r="C7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="19"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="12" t="s">
+      <c r="J7" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N16" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="21"/>
-    </row>
-    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="6" t="s">
+      <c r="I18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N18" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="1" t="str">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="2" t="str">
         <f>"(7)"</f>
         <v>(7)</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="19"/>
-    </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="11" t="s">
+      <c r="H22" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C24" s="1" t="s">
+      <c r="H23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="18"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="19"/>
-    </row>
-    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="11" t="s">
+      <c r="E27" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C29" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="1" t="s">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K31" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="22"/>
+      <c r="D32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K34" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J37" s="7"/>
+    </row>
+    <row r="38" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K31" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C39" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="21"/>
-      <c r="F32" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="19"/>
-    </row>
-    <row r="33" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="2" t="s">
+      <c r="B42" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="19"/>
+      <c r="D42" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H33" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I33" s="14" t="s">
+      <c r="H43" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J43" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="K43" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L43" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J33" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K34" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="19"/>
-      <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C39" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="19"/>
-      <c r="F42" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="19"/>
-    </row>
-    <row r="43" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="J43" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="K43" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="L43" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="M43" s="16" t="s">
+      <c r="M43" s="14" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="B17:F17"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="F32:K32"/>
     <mergeCell ref="F42:M42"/>
     <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="E7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
drobne poprawki w grafikach modeli
</commit_message>
<xml_diff>
--- a/first/TrafficSchool.xlsx
+++ b/first/TrafficSchool.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{07188FDE-DDF4-45C7-A62D-F895EAB70FF6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1A4CE95A-63DA-42F4-8179-B5EF215B24B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -496,10 +496,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,44 +791,45 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="7.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
@@ -848,7 +849,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
         <v>47</v>
       </c>
@@ -856,8 +857,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
@@ -871,15 +872,15 @@
       <c r="E7" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
         <v>33</v>
       </c>
@@ -901,23 +902,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20"/>
       <c r="G12" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -937,27 +938,27 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N16" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
@@ -980,7 +981,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
         <v>53</v>
       </c>
@@ -989,24 +990,24 @@
         <v>(7)</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>24</v>
       </c>
@@ -1029,7 +1030,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>53</v>
       </c>
@@ -1040,21 +1041,21 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
@@ -1068,7 +1069,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
         <v>53</v>
       </c>
@@ -1076,12 +1077,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K31" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
@@ -1095,16 +1096,16 @@
       <c r="F32" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="20"/>
       <c r="L32" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>48</v>
       </c>
@@ -1130,28 +1131,28 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K34" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20"/>
       <c r="F37" s="2" t="s">
         <v>60</v>
       </c>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>27</v>
       </c>
@@ -1168,38 +1169,38 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C39" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B42" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="19"/>
+      <c r="C42" s="20"/>
       <c r="D42" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="20"/>
       <c r="N42" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
         <v>52</v>
       </c>
@@ -1233,17 +1234,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="F42:M42"/>
+    <mergeCell ref="B37:E37"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="F42:M42"/>
-    <mergeCell ref="B37:E37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
mała zmiana w programie ze skryptem, usunięcie atrybutu Age, stworzenie triggera wyliczającego czas zakończenia lekcji praktycznej, skończenie uzupełniania bazy danymi
</commit_message>
<xml_diff>
--- a/first/TrafficSchool.xlsx
+++ b/first/TrafficSchool.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1A4CE95A-63DA-42F4-8179-B5EF215B24B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{32264025-43DD-499B-9B1B-64A2A6BAE7DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t>PERSON</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>TRAINEE</t>
-  </si>
-  <si>
-    <t>Age</t>
   </si>
   <si>
     <t>Theory</t>
@@ -496,10 +493,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,8 +798,7 @@
     <col min="3" max="3" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="11.140625" style="2" bestFit="1" customWidth="1"/>
@@ -816,106 +812,106 @@
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
+        <v>31</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="19"/>
       <c r="J7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -932,50 +928,50 @@
         <v>4</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="19"/>
       <c r="G17" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="I18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N18" s="16" t="s">
         <v>6</v>
@@ -983,7 +979,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F19" s="2" t="str">
         <f>"(7)"</f>
@@ -993,258 +989,254 @@
     <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="19"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="2" t="s">
-        <v>59</v>
+      <c r="G22" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>54</v>
+      <c r="G23" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="20"/>
+        <v>14</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K31" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="21" t="s">
         <v>29</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>30</v>
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="20"/>
+        <v>15</v>
+      </c>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="19"/>
       <c r="L32" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="H33" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K34" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="20"/>
+        <v>17</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="19"/>
       <c r="F37" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C39" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="C42" s="19"/>
       <c r="D42" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="20"/>
+        <v>20</v>
+      </c>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="19"/>
       <c r="N42" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I43" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K43" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="L43" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L43" s="15" t="s">
-        <v>24</v>
-      </c>
       <c r="M43" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="F42:M42"/>
-    <mergeCell ref="B37:E37"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="F42:M42"/>
+    <mergeCell ref="B37:E37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
okButton w nowych miastach/ulicach/starting_date i poczatek insertTrainee
</commit_message>
<xml_diff>
--- a/first/TrafficSchool.xlsx
+++ b/first/TrafficSchool.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{32264025-43DD-499B-9B1B-64A2A6BAE7DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{690643DB-7549-4EB2-917E-0C0458EAB47B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,16 +196,16 @@
     <t>emp Y</t>
   </si>
   <si>
-    <t>script N</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>scriptTRN N</t>
-  </si>
-  <si>
     <t>word_emp Y</t>
+  </si>
+  <si>
+    <t>scriptTRN Y</t>
+  </si>
+  <si>
+    <t>script Y</t>
   </si>
 </sst>
 </file>
@@ -493,10 +493,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,12 +817,12 @@
       <c r="B2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -862,18 +862,18 @@
         <v>9</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -906,10 +906,10 @@
       <c r="B12" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20"/>
       <c r="G12" s="2" t="s">
         <v>57</v>
       </c>
@@ -946,12 +946,12 @@
       <c r="B17" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -994,12 +994,12 @@
       <c r="B22" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1041,10 +1041,10 @@
       <c r="B27" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1083,18 +1083,18 @@
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F32" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="20"/>
       <c r="L32" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1136,11 +1136,11 @@
       <c r="B37" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20"/>
       <c r="F37" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J37" s="7"/>
     </row>
@@ -1174,22 +1174,22 @@
       <c r="B42" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="19"/>
+      <c r="C42" s="20"/>
       <c r="D42" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="20"/>
       <c r="N42" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1226,6 +1226,10 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="F42:M42"/>
+    <mergeCell ref="B37:E37"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B27:D27"/>
@@ -1233,10 +1237,6 @@
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="F42:M42"/>
-    <mergeCell ref="B37:E37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>